<commit_message>
Deploy codeforIATI/codelists to github.com/codeforIATI/codelists.git:gh-pages
</commit_message>
<xml_diff>
--- a/api/clv2/xlsx/fr/Sector.xlsx
+++ b/api/clv2/xlsx/fr/Sector.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="930">
   <si>
     <t>code</t>
   </si>
@@ -1309,57 +1309,150 @@
     <t>23010</t>
   </si>
   <si>
+    <t>Politique de l’énergie et gestion administrative</t>
+  </si>
+  <si>
+    <t>Politique de l’énergie, planification et programmes; aide aux ministères de l’énergie; renforcement des capacités institutionnelles et conseils; activités non spécifiées dans le domaine de l’énergie y compris les économies d’énergie.</t>
+  </si>
+  <si>
     <t>230</t>
   </si>
   <si>
     <t>23020</t>
   </si>
   <si>
+    <t>Production d’énergie (sources non renouvelables)</t>
+  </si>
+  <si>
+    <t>Centrales thermiques (lorsque la source de chaleur ne peut être déterminée); centrales alimentées au gaz et au charbon.</t>
+  </si>
+  <si>
     <t>23030</t>
   </si>
   <si>
+    <t>Production d’énergie (sources renouvelables)</t>
+  </si>
+  <si>
+    <t>Y compris politique et planification, programmes de développement, études et primes. Production de bois de chauffage et de charbon de bois devrait être incluse dans sylviculture (31261).</t>
+  </si>
+  <si>
     <t>23040</t>
   </si>
   <si>
+    <t>Transmission et distribution d’électricité</t>
+  </si>
+  <si>
+    <t>Distribution de la source d’énergie au consommateur; lignes de transmission.</t>
+  </si>
+  <si>
     <t>23050</t>
   </si>
   <si>
+    <t>Distribution de gaz</t>
+  </si>
+  <si>
+    <t>Distribution au consommateur.</t>
+  </si>
+  <si>
     <t>23061</t>
   </si>
   <si>
+    <t>Centrales alimentées au fuel</t>
+  </si>
+  <si>
+    <t>Y compris les centrales alimentées au gas-oil.</t>
+  </si>
+  <si>
     <t>23062</t>
   </si>
   <si>
+    <t>Centrales alimentées au gaz</t>
+  </si>
+  <si>
     <t>23063</t>
   </si>
   <si>
+    <t>Centrales alimentées au charbon</t>
+  </si>
+  <si>
     <t>23064</t>
   </si>
   <si>
+    <t>Centrales nucléaires</t>
+  </si>
+  <si>
+    <t>Y compris la sécurité nucléaire. L’aide visant à favoriser une utilisation pacifique de l’énergie nucléaire est comptabilisable dans l’APD. À titre d’exemples, on citera : la construction ou le déclassement de centrales nucléaires à des fins civiles, le développement ou la fourniture d’isotopes médicaux, l’irradiation des aliments et d’autres applications industrielles et commerciales. Sont par contre exclues les activités de recherche sur les armes nucléaires et les applications militaires de la technologie nucléaire.</t>
+  </si>
+  <si>
     <t>23065</t>
   </si>
   <si>
+    <t>Centrales et barrages hydroélectriques</t>
+  </si>
+  <si>
+    <t>Y compris les installations sur les barges.</t>
+  </si>
+  <si>
     <t>23066</t>
   </si>
   <si>
+    <t>Énergie géothermique</t>
+  </si>
+  <si>
     <t>23067</t>
   </si>
   <si>
+    <t>Énergie solaire</t>
+  </si>
+  <si>
+    <t>Y compris les cellules photovoltaïques et les pompes à énergie solaire.</t>
+  </si>
+  <si>
     <t>23068</t>
   </si>
   <si>
+    <t>Énergie éolienne</t>
+  </si>
+  <si>
+    <t>Énergie éolienne pour l’hydrodynamique et la production d’électricité.</t>
+  </si>
+  <si>
     <t>23069</t>
   </si>
   <si>
+    <t>Énergie marémotrice</t>
+  </si>
+  <si>
+    <t>Y compris la conversion de l’énergie thermique marine, la puissance des marées et des vagues.</t>
+  </si>
+  <si>
     <t>23070</t>
   </si>
   <si>
+    <t>Biomasse</t>
+  </si>
+  <si>
+    <t>Technologies de densification et utilisation de la biomasse pour la production d’énergie directe, y compris le gaz obtenu par fermentation de la canne à sucre et d’autres résidus végétaux, et par anaérobie.</t>
+  </si>
+  <si>
     <t>23081</t>
   </si>
   <si>
+    <t>Éducation et formation dans le domaine de l’énergie</t>
+  </si>
+  <si>
+    <t>Se rapporte à tous les sous-secteurs de l’énergie et à tous les niveaux de formation.</t>
+  </si>
+  <si>
     <t>23082</t>
   </si>
   <si>
+    <t>Recherche dans le domaine de l’énergie</t>
+  </si>
+  <si>
+    <t>Y compris inventaires et études.</t>
+  </si>
+  <si>
     <t>23110</t>
   </si>
   <si>
@@ -1402,9 +1495,6 @@
     <t>Recherche dans le domaine de l'énergie</t>
   </si>
   <si>
-    <t>Y compris inventaires et études.</t>
-  </si>
-  <si>
     <t>23183</t>
   </si>
   <si>
@@ -1438,18 +1528,12 @@
     <t>23230</t>
   </si>
   <si>
-    <t>Énergie solaire</t>
-  </si>
-  <si>
     <t>Solaire photovoltaïque, thermodynamique, chauffage solaire.</t>
   </si>
   <si>
     <t>23240</t>
   </si>
   <si>
-    <t>Énergie éolienne</t>
-  </si>
-  <si>
     <t>Éoliennes de pompage et production d’électricité.</t>
   </si>
   <si>
@@ -1465,9 +1549,6 @@
     <t>23260</t>
   </si>
   <si>
-    <t>Énergie géothermique</t>
-  </si>
-  <si>
     <t>Application de l’énergie géothermique pour produire de l’électricité ou production de chaleur à usage agricole, etc.</t>
   </si>
   <si>
@@ -1550,9 +1631,6 @@
   </si>
   <si>
     <t>23510</t>
-  </si>
-  <si>
-    <t>Centrales nucléaires</t>
   </si>
   <si>
     <t>Dont sûreté nucléaire.</t>
@@ -5447,8 +5525,14 @@
       <c r="A144" t="s">
         <v>430</v>
       </c>
+      <c r="B144" t="s">
+        <v>431</v>
+      </c>
+      <c r="C144" t="s">
+        <v>432</v>
+      </c>
       <c r="D144" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F144" t="s">
         <v>195</v>
@@ -5456,10 +5540,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>432</v>
+        <v>434</v>
+      </c>
+      <c r="B145" t="s">
+        <v>435</v>
+      </c>
+      <c r="C145" t="s">
+        <v>436</v>
       </c>
       <c r="D145" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F145" t="s">
         <v>195</v>
@@ -5467,10 +5557,16 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
+        <v>437</v>
+      </c>
+      <c r="B146" t="s">
+        <v>438</v>
+      </c>
+      <c r="C146" t="s">
+        <v>439</v>
+      </c>
+      <c r="D146" t="s">
         <v>433</v>
-      </c>
-      <c r="D146" t="s">
-        <v>431</v>
       </c>
       <c r="F146" t="s">
         <v>195</v>
@@ -5478,10 +5574,16 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>434</v>
+        <v>440</v>
+      </c>
+      <c r="B147" t="s">
+        <v>441</v>
+      </c>
+      <c r="C147" t="s">
+        <v>442</v>
       </c>
       <c r="D147" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F147" t="s">
         <v>195</v>
@@ -5489,10 +5591,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>435</v>
+        <v>443</v>
+      </c>
+      <c r="B148" t="s">
+        <v>444</v>
+      </c>
+      <c r="C148" t="s">
+        <v>445</v>
       </c>
       <c r="D148" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F148" t="s">
         <v>195</v>
@@ -5500,10 +5608,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>436</v>
+        <v>446</v>
+      </c>
+      <c r="B149" t="s">
+        <v>447</v>
+      </c>
+      <c r="C149" t="s">
+        <v>448</v>
       </c>
       <c r="D149" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F149" t="s">
         <v>195</v>
@@ -5511,10 +5625,13 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>437</v>
+        <v>449</v>
+      </c>
+      <c r="B150" t="s">
+        <v>450</v>
       </c>
       <c r="D150" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F150" t="s">
         <v>195</v>
@@ -5522,10 +5639,13 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>438</v>
+        <v>451</v>
+      </c>
+      <c r="B151" t="s">
+        <v>452</v>
       </c>
       <c r="D151" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F151" t="s">
         <v>195</v>
@@ -5533,10 +5653,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>439</v>
+        <v>453</v>
+      </c>
+      <c r="B152" t="s">
+        <v>454</v>
+      </c>
+      <c r="C152" t="s">
+        <v>455</v>
       </c>
       <c r="D152" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F152" t="s">
         <v>195</v>
@@ -5544,10 +5670,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>440</v>
+        <v>456</v>
+      </c>
+      <c r="B153" t="s">
+        <v>457</v>
+      </c>
+      <c r="C153" t="s">
+        <v>458</v>
       </c>
       <c r="D153" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F153" t="s">
         <v>195</v>
@@ -5555,10 +5687,13 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>441</v>
+        <v>459</v>
+      </c>
+      <c r="B154" t="s">
+        <v>460</v>
       </c>
       <c r="D154" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F154" t="s">
         <v>195</v>
@@ -5566,10 +5701,16 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>442</v>
+        <v>461</v>
+      </c>
+      <c r="B155" t="s">
+        <v>462</v>
+      </c>
+      <c r="C155" t="s">
+        <v>463</v>
       </c>
       <c r="D155" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F155" t="s">
         <v>195</v>
@@ -5577,10 +5718,16 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>443</v>
+        <v>464</v>
+      </c>
+      <c r="B156" t="s">
+        <v>465</v>
+      </c>
+      <c r="C156" t="s">
+        <v>466</v>
       </c>
       <c r="D156" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F156" t="s">
         <v>195</v>
@@ -5588,10 +5735,16 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>444</v>
+        <v>467</v>
+      </c>
+      <c r="B157" t="s">
+        <v>468</v>
+      </c>
+      <c r="C157" t="s">
+        <v>469</v>
       </c>
       <c r="D157" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F157" t="s">
         <v>195</v>
@@ -5599,10 +5752,16 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>445</v>
+        <v>470</v>
+      </c>
+      <c r="B158" t="s">
+        <v>471</v>
+      </c>
+      <c r="C158" t="s">
+        <v>472</v>
       </c>
       <c r="D158" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F158" t="s">
         <v>195</v>
@@ -5610,10 +5769,16 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>446</v>
+        <v>473</v>
+      </c>
+      <c r="B159" t="s">
+        <v>474</v>
+      </c>
+      <c r="C159" t="s">
+        <v>475</v>
       </c>
       <c r="D159" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F159" t="s">
         <v>195</v>
@@ -5621,10 +5786,16 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>447</v>
+        <v>476</v>
+      </c>
+      <c r="B160" t="s">
+        <v>477</v>
+      </c>
+      <c r="C160" t="s">
+        <v>478</v>
       </c>
       <c r="D160" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F160" t="s">
         <v>195</v>
@@ -5632,16 +5803,16 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="B161" t="s">
-        <v>449</v>
+        <v>480</v>
       </c>
       <c r="C161" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D161" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F161" t="s">
         <v>10</v>
@@ -5649,13 +5820,13 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="B162" t="s">
-        <v>453</v>
+        <v>484</v>
       </c>
       <c r="D162" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F162" t="s">
         <v>10</v>
@@ -5663,16 +5834,16 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="B163" t="s">
-        <v>455</v>
+        <v>486</v>
       </c>
       <c r="C163" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="D163" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
@@ -5680,16 +5851,16 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>457</v>
+        <v>488</v>
       </c>
       <c r="B164" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C164" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="D164" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F164" t="s">
         <v>10</v>
@@ -5697,16 +5868,16 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="B165" t="s">
-        <v>461</v>
+        <v>492</v>
       </c>
       <c r="C165" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="D165" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -5714,16 +5885,16 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="B166" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="C166" t="s">
-        <v>465</v>
+        <v>495</v>
       </c>
       <c r="D166" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
@@ -5731,16 +5902,16 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>466</v>
+        <v>496</v>
       </c>
       <c r="B167" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
       <c r="C167" t="s">
-        <v>468</v>
+        <v>498</v>
       </c>
       <c r="D167" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -5748,16 +5919,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="B168" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="C168" t="s">
-        <v>472</v>
+        <v>502</v>
       </c>
       <c r="D168" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F168" t="s">
         <v>10</v>
@@ -5765,16 +5936,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="B169" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="C169" t="s">
-        <v>475</v>
+        <v>504</v>
       </c>
       <c r="D169" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -5782,16 +5953,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>476</v>
+        <v>505</v>
       </c>
       <c r="B170" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C170" t="s">
-        <v>478</v>
+        <v>506</v>
       </c>
       <c r="D170" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F170" t="s">
         <v>10</v>
@@ -5799,16 +5970,16 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>479</v>
+        <v>507</v>
       </c>
       <c r="B171" t="s">
-        <v>480</v>
+        <v>508</v>
       </c>
       <c r="C171" t="s">
-        <v>481</v>
+        <v>509</v>
       </c>
       <c r="D171" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F171" t="s">
         <v>10</v>
@@ -5816,16 +5987,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>482</v>
+        <v>510</v>
       </c>
       <c r="B172" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
       <c r="C172" t="s">
-        <v>484</v>
+        <v>511</v>
       </c>
       <c r="D172" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F172" t="s">
         <v>10</v>
@@ -5833,16 +6004,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>485</v>
+        <v>512</v>
       </c>
       <c r="B173" t="s">
-        <v>486</v>
+        <v>513</v>
       </c>
       <c r="C173" t="s">
-        <v>487</v>
+        <v>514</v>
       </c>
       <c r="D173" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -5850,16 +6021,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>488</v>
+        <v>515</v>
       </c>
       <c r="B174" t="s">
-        <v>489</v>
+        <v>516</v>
       </c>
       <c r="C174" t="s">
-        <v>490</v>
+        <v>517</v>
       </c>
       <c r="D174" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F174" t="s">
         <v>10</v>
@@ -5867,16 +6038,16 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>492</v>
+        <v>519</v>
       </c>
       <c r="B175" t="s">
-        <v>493</v>
+        <v>520</v>
       </c>
       <c r="C175" t="s">
-        <v>494</v>
+        <v>521</v>
       </c>
       <c r="D175" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F175" t="s">
         <v>10</v>
@@ -5884,16 +6055,16 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>495</v>
+        <v>522</v>
       </c>
       <c r="B176" t="s">
-        <v>496</v>
+        <v>523</v>
       </c>
       <c r="C176" t="s">
-        <v>497</v>
+        <v>524</v>
       </c>
       <c r="D176" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -5901,16 +6072,16 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>498</v>
+        <v>525</v>
       </c>
       <c r="B177" t="s">
-        <v>499</v>
+        <v>526</v>
       </c>
       <c r="C177" t="s">
-        <v>500</v>
+        <v>527</v>
       </c>
       <c r="D177" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F177" t="s">
         <v>10</v>
@@ -5918,16 +6089,16 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>501</v>
+        <v>528</v>
       </c>
       <c r="B178" t="s">
-        <v>502</v>
+        <v>529</v>
       </c>
       <c r="C178" t="s">
-        <v>503</v>
+        <v>530</v>
       </c>
       <c r="D178" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
@@ -5935,16 +6106,16 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>504</v>
+        <v>531</v>
       </c>
       <c r="B179" t="s">
-        <v>505</v>
+        <v>532</v>
       </c>
       <c r="C179" t="s">
-        <v>506</v>
+        <v>533</v>
       </c>
       <c r="D179" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -5952,16 +6123,16 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>507</v>
+        <v>534</v>
       </c>
       <c r="B180" t="s">
-        <v>508</v>
+        <v>535</v>
       </c>
       <c r="C180" t="s">
-        <v>509</v>
+        <v>536</v>
       </c>
       <c r="D180" t="s">
-        <v>510</v>
+        <v>537</v>
       </c>
       <c r="F180" t="s">
         <v>10</v>
@@ -5969,16 +6140,16 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>511</v>
+        <v>538</v>
       </c>
       <c r="B181" t="s">
-        <v>512</v>
+        <v>454</v>
       </c>
       <c r="C181" t="s">
-        <v>513</v>
+        <v>539</v>
       </c>
       <c r="D181" t="s">
-        <v>514</v>
+        <v>540</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>
@@ -5986,16 +6157,16 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>515</v>
+        <v>541</v>
       </c>
       <c r="B182" t="s">
-        <v>516</v>
+        <v>542</v>
       </c>
       <c r="C182" t="s">
-        <v>517</v>
+        <v>543</v>
       </c>
       <c r="D182" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="F182" t="s">
         <v>10</v>
@@ -6003,16 +6174,16 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
-        <v>519</v>
+        <v>545</v>
       </c>
       <c r="B183" t="s">
-        <v>520</v>
+        <v>546</v>
       </c>
       <c r="C183" t="s">
-        <v>521</v>
+        <v>547</v>
       </c>
       <c r="D183" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="F183" t="s">
         <v>10</v>
@@ -6020,16 +6191,16 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>522</v>
+        <v>548</v>
       </c>
       <c r="B184" t="s">
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="C184" t="s">
-        <v>524</v>
+        <v>550</v>
       </c>
       <c r="D184" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="F184" t="s">
         <v>10</v>
@@ -6037,16 +6208,16 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
-        <v>525</v>
+        <v>551</v>
       </c>
       <c r="B185" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
       <c r="C185" t="s">
-        <v>527</v>
+        <v>553</v>
       </c>
       <c r="D185" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="F185" t="s">
         <v>10</v>
@@ -6054,16 +6225,16 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>528</v>
+        <v>554</v>
       </c>
       <c r="B186" t="s">
-        <v>529</v>
+        <v>555</v>
       </c>
       <c r="C186" t="s">
-        <v>530</v>
+        <v>556</v>
       </c>
       <c r="D186" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F186" t="s">
         <v>10</v>
@@ -6071,16 +6242,16 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>532</v>
+        <v>558</v>
       </c>
       <c r="B187" t="s">
-        <v>533</v>
+        <v>559</v>
       </c>
       <c r="C187" t="s">
-        <v>534</v>
+        <v>560</v>
       </c>
       <c r="D187" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F187" t="s">
         <v>10</v>
@@ -6088,16 +6259,16 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>535</v>
+        <v>561</v>
       </c>
       <c r="B188" t="s">
-        <v>536</v>
+        <v>562</v>
       </c>
       <c r="C188" t="s">
-        <v>537</v>
+        <v>563</v>
       </c>
       <c r="D188" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F188" t="s">
         <v>10</v>
@@ -6105,16 +6276,16 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" t="s">
-        <v>538</v>
+        <v>564</v>
       </c>
       <c r="B189" t="s">
-        <v>539</v>
+        <v>565</v>
       </c>
       <c r="C189" t="s">
-        <v>540</v>
+        <v>566</v>
       </c>
       <c r="D189" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F189" t="s">
         <v>10</v>
@@ -6122,16 +6293,16 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>541</v>
+        <v>567</v>
       </c>
       <c r="B190" t="s">
-        <v>542</v>
+        <v>568</v>
       </c>
       <c r="C190" t="s">
-        <v>543</v>
+        <v>569</v>
       </c>
       <c r="D190" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
@@ -6139,13 +6310,13 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>544</v>
+        <v>570</v>
       </c>
       <c r="B191" t="s">
-        <v>545</v>
+        <v>571</v>
       </c>
       <c r="D191" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="F191" t="s">
         <v>10</v>
@@ -6153,16 +6324,16 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>546</v>
+        <v>572</v>
       </c>
       <c r="B192" t="s">
-        <v>547</v>
+        <v>573</v>
       </c>
       <c r="C192" t="s">
-        <v>548</v>
+        <v>574</v>
       </c>
       <c r="D192" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="F192" t="s">
         <v>10</v>
@@ -6170,16 +6341,16 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>550</v>
+        <v>576</v>
       </c>
       <c r="B193" t="s">
-        <v>551</v>
+        <v>577</v>
       </c>
       <c r="C193" t="s">
-        <v>552</v>
+        <v>578</v>
       </c>
       <c r="D193" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="F193" t="s">
         <v>10</v>
@@ -6187,13 +6358,13 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" t="s">
-        <v>553</v>
+        <v>579</v>
       </c>
       <c r="B194" t="s">
-        <v>554</v>
+        <v>580</v>
       </c>
       <c r="D194" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="F194" t="s">
         <v>10</v>
@@ -6201,13 +6372,13 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>555</v>
+        <v>581</v>
       </c>
       <c r="B195" t="s">
-        <v>556</v>
+        <v>582</v>
       </c>
       <c r="D195" t="s">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="F195" t="s">
         <v>10</v>
@@ -6215,16 +6386,16 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>557</v>
+        <v>583</v>
       </c>
       <c r="B196" t="s">
-        <v>558</v>
+        <v>584</v>
       </c>
       <c r="C196" t="s">
-        <v>559</v>
+        <v>585</v>
       </c>
       <c r="D196" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F196" t="s">
         <v>10</v>
@@ -6232,16 +6403,16 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
-        <v>561</v>
+        <v>587</v>
       </c>
       <c r="B197" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
       <c r="C197" t="s">
-        <v>563</v>
+        <v>589</v>
       </c>
       <c r="D197" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F197" t="s">
         <v>10</v>
@@ -6249,16 +6420,16 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" t="s">
-        <v>564</v>
+        <v>590</v>
       </c>
       <c r="B198" t="s">
-        <v>565</v>
+        <v>591</v>
       </c>
       <c r="C198" t="s">
-        <v>566</v>
+        <v>592</v>
       </c>
       <c r="D198" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F198" t="s">
         <v>10</v>
@@ -6266,16 +6437,16 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" t="s">
-        <v>567</v>
+        <v>593</v>
       </c>
       <c r="B199" t="s">
-        <v>568</v>
+        <v>594</v>
       </c>
       <c r="C199" t="s">
-        <v>569</v>
+        <v>595</v>
       </c>
       <c r="D199" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F199" t="s">
         <v>10</v>
@@ -6283,16 +6454,16 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>570</v>
+        <v>596</v>
       </c>
       <c r="B200" t="s">
-        <v>571</v>
+        <v>597</v>
       </c>
       <c r="C200" t="s">
-        <v>572</v>
+        <v>598</v>
       </c>
       <c r="D200" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F200" t="s">
         <v>10</v>
@@ -6300,16 +6471,16 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>573</v>
+        <v>599</v>
       </c>
       <c r="B201" t="s">
-        <v>574</v>
+        <v>600</v>
       </c>
       <c r="C201" t="s">
-        <v>575</v>
+        <v>601</v>
       </c>
       <c r="D201" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F201" t="s">
         <v>10</v>
@@ -6317,16 +6488,16 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>576</v>
+        <v>602</v>
       </c>
       <c r="B202" t="s">
-        <v>577</v>
+        <v>603</v>
       </c>
       <c r="C202" t="s">
-        <v>578</v>
+        <v>604</v>
       </c>
       <c r="D202" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F202" t="s">
         <v>10</v>
@@ -6334,16 +6505,16 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="B203" t="s">
-        <v>580</v>
+        <v>606</v>
       </c>
       <c r="C203" t="s">
-        <v>581</v>
+        <v>607</v>
       </c>
       <c r="D203" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F203" t="s">
         <v>10</v>
@@ -6351,16 +6522,16 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" t="s">
-        <v>582</v>
+        <v>608</v>
       </c>
       <c r="B204" t="s">
-        <v>583</v>
+        <v>609</v>
       </c>
       <c r="C204" t="s">
-        <v>584</v>
+        <v>610</v>
       </c>
       <c r="D204" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F204" t="s">
         <v>10</v>
@@ -6368,16 +6539,16 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" t="s">
-        <v>585</v>
+        <v>611</v>
       </c>
       <c r="B205" t="s">
+        <v>612</v>
+      </c>
+      <c r="C205" t="s">
+        <v>613</v>
+      </c>
+      <c r="D205" t="s">
         <v>586</v>
-      </c>
-      <c r="C205" t="s">
-        <v>587</v>
-      </c>
-      <c r="D205" t="s">
-        <v>560</v>
       </c>
       <c r="F205" t="s">
         <v>10</v>
@@ -6385,16 +6556,16 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" t="s">
-        <v>588</v>
+        <v>614</v>
       </c>
       <c r="B206" t="s">
-        <v>589</v>
+        <v>615</v>
       </c>
       <c r="C206" t="s">
-        <v>590</v>
+        <v>616</v>
       </c>
       <c r="D206" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F206" t="s">
         <v>10</v>
@@ -6402,13 +6573,13 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="B207" t="s">
-        <v>592</v>
+        <v>618</v>
       </c>
       <c r="D207" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F207" t="s">
         <v>10</v>
@@ -6416,16 +6587,16 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" t="s">
-        <v>593</v>
+        <v>619</v>
       </c>
       <c r="B208" t="s">
-        <v>594</v>
+        <v>620</v>
       </c>
       <c r="C208" t="s">
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="D208" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F208" t="s">
         <v>10</v>
@@ -6433,16 +6604,16 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" t="s">
-        <v>596</v>
+        <v>622</v>
       </c>
       <c r="B209" t="s">
-        <v>597</v>
+        <v>623</v>
       </c>
       <c r="C209" t="s">
-        <v>598</v>
+        <v>624</v>
       </c>
       <c r="D209" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F209" t="s">
         <v>10</v>
@@ -6450,16 +6621,16 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
-        <v>599</v>
+        <v>625</v>
       </c>
       <c r="B210" t="s">
-        <v>600</v>
+        <v>626</v>
       </c>
       <c r="C210" t="s">
-        <v>601</v>
+        <v>627</v>
       </c>
       <c r="D210" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F210" t="s">
         <v>10</v>
@@ -6467,16 +6638,16 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
-        <v>602</v>
+        <v>628</v>
       </c>
       <c r="B211" t="s">
-        <v>603</v>
+        <v>629</v>
       </c>
       <c r="C211" t="s">
-        <v>604</v>
+        <v>630</v>
       </c>
       <c r="D211" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F211" t="s">
         <v>10</v>
@@ -6484,16 +6655,16 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" t="s">
-        <v>605</v>
+        <v>631</v>
       </c>
       <c r="B212" t="s">
-        <v>606</v>
+        <v>632</v>
       </c>
       <c r="C212" t="s">
-        <v>607</v>
+        <v>633</v>
       </c>
       <c r="D212" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F212" t="s">
         <v>10</v>
@@ -6501,16 +6672,16 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" t="s">
-        <v>608</v>
+        <v>634</v>
       </c>
       <c r="B213" t="s">
-        <v>609</v>
+        <v>635</v>
       </c>
       <c r="C213" t="s">
-        <v>610</v>
+        <v>636</v>
       </c>
       <c r="D213" t="s">
-        <v>560</v>
+        <v>586</v>
       </c>
       <c r="F213" t="s">
         <v>10</v>
@@ -6518,16 +6689,16 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" t="s">
-        <v>611</v>
+        <v>637</v>
       </c>
       <c r="B214" t="s">
-        <v>612</v>
+        <v>638</v>
       </c>
       <c r="C214" t="s">
-        <v>613</v>
+        <v>639</v>
       </c>
       <c r="D214" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F214" t="s">
         <v>10</v>
@@ -6535,16 +6706,16 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" t="s">
-        <v>615</v>
+        <v>641</v>
       </c>
       <c r="B215" t="s">
-        <v>616</v>
+        <v>642</v>
       </c>
       <c r="C215" t="s">
-        <v>617</v>
+        <v>643</v>
       </c>
       <c r="D215" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F215" t="s">
         <v>10</v>
@@ -6552,16 +6723,16 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
       <c r="B216" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="C216" t="s">
-        <v>620</v>
+        <v>646</v>
       </c>
       <c r="D216" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F216" t="s">
         <v>10</v>
@@ -6569,13 +6740,13 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" t="s">
-        <v>621</v>
+        <v>647</v>
       </c>
       <c r="B217" t="s">
-        <v>622</v>
+        <v>648</v>
       </c>
       <c r="D217" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F217" t="s">
         <v>10</v>
@@ -6583,16 +6754,16 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>623</v>
+        <v>649</v>
       </c>
       <c r="B218" t="s">
-        <v>624</v>
+        <v>650</v>
       </c>
       <c r="C218" t="s">
-        <v>625</v>
+        <v>651</v>
       </c>
       <c r="D218" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F218" t="s">
         <v>10</v>
@@ -6600,13 +6771,13 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" t="s">
-        <v>626</v>
+        <v>652</v>
       </c>
       <c r="B219" t="s">
-        <v>627</v>
+        <v>653</v>
       </c>
       <c r="D219" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
       <c r="F219" t="s">
         <v>10</v>
@@ -6614,16 +6785,16 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" t="s">
-        <v>628</v>
+        <v>654</v>
       </c>
       <c r="B220" t="s">
-        <v>629</v>
+        <v>655</v>
       </c>
       <c r="C220" t="s">
-        <v>630</v>
+        <v>656</v>
       </c>
       <c r="D220" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="F220" t="s">
         <v>10</v>
@@ -6631,16 +6802,16 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" t="s">
-        <v>632</v>
+        <v>658</v>
       </c>
       <c r="B221" t="s">
-        <v>633</v>
+        <v>659</v>
       </c>
       <c r="C221" t="s">
-        <v>634</v>
+        <v>660</v>
       </c>
       <c r="D221" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="F221" t="s">
         <v>10</v>
@@ -6648,13 +6819,13 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" t="s">
-        <v>635</v>
+        <v>661</v>
       </c>
       <c r="B222" t="s">
-        <v>636</v>
+        <v>662</v>
       </c>
       <c r="D222" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="F222" t="s">
         <v>10</v>
@@ -6662,16 +6833,16 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" t="s">
-        <v>637</v>
+        <v>663</v>
       </c>
       <c r="B223" t="s">
-        <v>638</v>
+        <v>664</v>
       </c>
       <c r="C223" t="s">
-        <v>639</v>
+        <v>665</v>
       </c>
       <c r="D223" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="F223" t="s">
         <v>10</v>
@@ -6679,16 +6850,16 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
-        <v>640</v>
+        <v>666</v>
       </c>
       <c r="B224" t="s">
-        <v>641</v>
+        <v>667</v>
       </c>
       <c r="C224" t="s">
-        <v>642</v>
+        <v>668</v>
       </c>
       <c r="D224" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="F224" t="s">
         <v>10</v>
@@ -6696,16 +6867,16 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
-        <v>643</v>
+        <v>669</v>
       </c>
       <c r="B225" t="s">
-        <v>644</v>
+        <v>670</v>
       </c>
       <c r="C225" t="s">
-        <v>645</v>
+        <v>671</v>
       </c>
       <c r="D225" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F225" t="s">
         <v>10</v>
@@ -6713,13 +6884,13 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
-        <v>647</v>
+        <v>673</v>
       </c>
       <c r="B226" t="s">
-        <v>648</v>
+        <v>674</v>
       </c>
       <c r="D226" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F226" t="s">
         <v>10</v>
@@ -6727,16 +6898,16 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
-        <v>649</v>
+        <v>675</v>
       </c>
       <c r="B227" t="s">
-        <v>650</v>
+        <v>676</v>
       </c>
       <c r="C227" t="s">
-        <v>651</v>
+        <v>677</v>
       </c>
       <c r="D227" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F227" t="s">
         <v>10</v>
@@ -6744,13 +6915,13 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
-        <v>652</v>
+        <v>678</v>
       </c>
       <c r="B228" t="s">
-        <v>653</v>
+        <v>679</v>
       </c>
       <c r="D228" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F228" t="s">
         <v>10</v>
@@ -6758,16 +6929,16 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" t="s">
-        <v>654</v>
+        <v>680</v>
       </c>
       <c r="B229" t="s">
-        <v>655</v>
+        <v>681</v>
       </c>
       <c r="C229" t="s">
-        <v>656</v>
+        <v>682</v>
       </c>
       <c r="D229" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F229" t="s">
         <v>10</v>
@@ -6775,16 +6946,16 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" t="s">
-        <v>657</v>
+        <v>683</v>
       </c>
       <c r="B230" t="s">
-        <v>658</v>
+        <v>684</v>
       </c>
       <c r="C230" t="s">
-        <v>659</v>
+        <v>685</v>
       </c>
       <c r="D230" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F230" t="s">
         <v>10</v>
@@ -6792,16 +6963,16 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" t="s">
-        <v>660</v>
+        <v>686</v>
       </c>
       <c r="B231" t="s">
-        <v>661</v>
+        <v>687</v>
       </c>
       <c r="C231" t="s">
-        <v>662</v>
+        <v>688</v>
       </c>
       <c r="D231" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F231" t="s">
         <v>10</v>
@@ -6809,16 +6980,16 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>663</v>
+        <v>689</v>
       </c>
       <c r="B232" t="s">
-        <v>664</v>
+        <v>690</v>
       </c>
       <c r="C232" t="s">
-        <v>665</v>
+        <v>691</v>
       </c>
       <c r="D232" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F232" t="s">
         <v>10</v>
@@ -6826,13 +6997,13 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>666</v>
+        <v>692</v>
       </c>
       <c r="B233" t="s">
-        <v>667</v>
+        <v>693</v>
       </c>
       <c r="D233" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F233" t="s">
         <v>10</v>
@@ -6840,13 +7011,13 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>668</v>
+        <v>694</v>
       </c>
       <c r="B234" t="s">
-        <v>669</v>
+        <v>695</v>
       </c>
       <c r="D234" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F234" t="s">
         <v>10</v>
@@ -6854,16 +7025,16 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>670</v>
+        <v>696</v>
       </c>
       <c r="B235" t="s">
-        <v>671</v>
+        <v>697</v>
       </c>
       <c r="C235" t="s">
+        <v>698</v>
+      </c>
+      <c r="D235" t="s">
         <v>672</v>
-      </c>
-      <c r="D235" t="s">
-        <v>646</v>
       </c>
       <c r="F235" t="s">
         <v>10</v>
@@ -6871,16 +7042,16 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>673</v>
+        <v>699</v>
       </c>
       <c r="B236" t="s">
-        <v>674</v>
+        <v>700</v>
       </c>
       <c r="C236" t="s">
-        <v>675</v>
+        <v>701</v>
       </c>
       <c r="D236" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F236" t="s">
         <v>10</v>
@@ -6888,16 +7059,16 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
-        <v>676</v>
+        <v>702</v>
       </c>
       <c r="B237" t="s">
-        <v>677</v>
+        <v>703</v>
       </c>
       <c r="C237" t="s">
-        <v>678</v>
+        <v>704</v>
       </c>
       <c r="D237" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F237" t="s">
         <v>10</v>
@@ -6905,13 +7076,13 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" t="s">
-        <v>679</v>
+        <v>705</v>
       </c>
       <c r="B238" t="s">
-        <v>680</v>
+        <v>706</v>
       </c>
       <c r="D238" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F238" t="s">
         <v>10</v>
@@ -6919,16 +7090,16 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" t="s">
-        <v>681</v>
+        <v>707</v>
       </c>
       <c r="B239" t="s">
-        <v>682</v>
+        <v>708</v>
       </c>
       <c r="C239" t="s">
-        <v>683</v>
+        <v>709</v>
       </c>
       <c r="D239" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F239" t="s">
         <v>10</v>
@@ -6936,16 +7107,16 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" t="s">
-        <v>684</v>
+        <v>710</v>
       </c>
       <c r="B240" t="s">
-        <v>685</v>
+        <v>711</v>
       </c>
       <c r="C240" t="s">
-        <v>686</v>
+        <v>712</v>
       </c>
       <c r="D240" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F240" t="s">
         <v>10</v>
@@ -6953,16 +7124,16 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" t="s">
-        <v>687</v>
+        <v>713</v>
       </c>
       <c r="B241" t="s">
-        <v>688</v>
+        <v>714</v>
       </c>
       <c r="C241" t="s">
-        <v>689</v>
+        <v>715</v>
       </c>
       <c r="D241" t="s">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="F241" t="s">
         <v>10</v>
@@ -6970,16 +7141,16 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" t="s">
-        <v>690</v>
+        <v>716</v>
       </c>
       <c r="B242" t="s">
-        <v>691</v>
+        <v>717</v>
       </c>
       <c r="C242" t="s">
-        <v>692</v>
+        <v>718</v>
       </c>
       <c r="D242" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F242" t="s">
         <v>10</v>
@@ -6987,16 +7158,16 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" t="s">
-        <v>694</v>
+        <v>720</v>
       </c>
       <c r="B243" t="s">
-        <v>695</v>
+        <v>721</v>
       </c>
       <c r="C243" t="s">
-        <v>696</v>
+        <v>722</v>
       </c>
       <c r="D243" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F243" t="s">
         <v>10</v>
@@ -7004,16 +7175,16 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" t="s">
-        <v>697</v>
+        <v>723</v>
       </c>
       <c r="B244" t="s">
-        <v>698</v>
+        <v>724</v>
       </c>
       <c r="C244" t="s">
-        <v>699</v>
+        <v>725</v>
       </c>
       <c r="D244" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F244" t="s">
         <v>10</v>
@@ -7021,16 +7192,16 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" t="s">
-        <v>700</v>
+        <v>726</v>
       </c>
       <c r="B245" t="s">
-        <v>701</v>
+        <v>727</v>
       </c>
       <c r="C245" t="s">
-        <v>702</v>
+        <v>728</v>
       </c>
       <c r="D245" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F245" t="s">
         <v>10</v>
@@ -7038,16 +7209,16 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" t="s">
-        <v>703</v>
+        <v>729</v>
       </c>
       <c r="B246" t="s">
-        <v>704</v>
+        <v>730</v>
       </c>
       <c r="C246" t="s">
-        <v>705</v>
+        <v>731</v>
       </c>
       <c r="D246" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F246" t="s">
         <v>10</v>
@@ -7055,16 +7226,16 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" t="s">
-        <v>706</v>
+        <v>732</v>
       </c>
       <c r="B247" t="s">
-        <v>707</v>
+        <v>733</v>
       </c>
       <c r="C247" t="s">
-        <v>708</v>
+        <v>734</v>
       </c>
       <c r="D247" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F247" t="s">
         <v>10</v>
@@ -7072,16 +7243,16 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" t="s">
-        <v>709</v>
+        <v>735</v>
       </c>
       <c r="B248" t="s">
-        <v>710</v>
+        <v>736</v>
       </c>
       <c r="C248" t="s">
-        <v>711</v>
+        <v>737</v>
       </c>
       <c r="D248" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F248" t="s">
         <v>10</v>
@@ -7089,16 +7260,16 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
-        <v>712</v>
+        <v>738</v>
       </c>
       <c r="B249" t="s">
-        <v>713</v>
+        <v>739</v>
       </c>
       <c r="C249" t="s">
-        <v>714</v>
+        <v>740</v>
       </c>
       <c r="D249" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F249" t="s">
         <v>10</v>
@@ -7106,16 +7277,16 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" t="s">
-        <v>715</v>
+        <v>741</v>
       </c>
       <c r="B250" t="s">
-        <v>716</v>
+        <v>742</v>
       </c>
       <c r="C250" t="s">
-        <v>717</v>
+        <v>743</v>
       </c>
       <c r="D250" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F250" t="s">
         <v>10</v>
@@ -7123,16 +7294,16 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" t="s">
-        <v>718</v>
+        <v>744</v>
       </c>
       <c r="B251" t="s">
+        <v>745</v>
+      </c>
+      <c r="C251" t="s">
+        <v>746</v>
+      </c>
+      <c r="D251" t="s">
         <v>719</v>
-      </c>
-      <c r="C251" t="s">
-        <v>720</v>
-      </c>
-      <c r="D251" t="s">
-        <v>693</v>
       </c>
       <c r="F251" t="s">
         <v>10</v>
@@ -7140,16 +7311,16 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" t="s">
-        <v>721</v>
+        <v>747</v>
       </c>
       <c r="B252" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
       <c r="C252" t="s">
-        <v>723</v>
+        <v>749</v>
       </c>
       <c r="D252" t="s">
-        <v>724</v>
+        <v>750</v>
       </c>
       <c r="F252" t="s">
         <v>10</v>
@@ -7157,16 +7328,16 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" t="s">
-        <v>725</v>
+        <v>751</v>
       </c>
       <c r="B253" t="s">
-        <v>726</v>
+        <v>752</v>
       </c>
       <c r="C253" t="s">
-        <v>727</v>
+        <v>753</v>
       </c>
       <c r="D253" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F253" t="s">
         <v>10</v>
@@ -7174,16 +7345,16 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" t="s">
-        <v>729</v>
+        <v>755</v>
       </c>
       <c r="B254" t="s">
-        <v>730</v>
+        <v>756</v>
       </c>
       <c r="C254" t="s">
-        <v>731</v>
+        <v>757</v>
       </c>
       <c r="D254" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F254" t="s">
         <v>10</v>
@@ -7191,16 +7362,16 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" t="s">
-        <v>732</v>
+        <v>758</v>
       </c>
       <c r="B255" t="s">
-        <v>733</v>
+        <v>759</v>
       </c>
       <c r="C255" t="s">
-        <v>734</v>
+        <v>760</v>
       </c>
       <c r="D255" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F255" t="s">
         <v>10</v>
@@ -7208,16 +7379,16 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" t="s">
-        <v>735</v>
+        <v>761</v>
       </c>
       <c r="B256" t="s">
-        <v>736</v>
+        <v>762</v>
       </c>
       <c r="C256" t="s">
-        <v>737</v>
+        <v>763</v>
       </c>
       <c r="D256" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F256" t="s">
         <v>10</v>
@@ -7225,16 +7396,16 @@
     </row>
     <row r="257" spans="1:6">
       <c r="A257" t="s">
-        <v>738</v>
+        <v>764</v>
       </c>
       <c r="B257" t="s">
-        <v>739</v>
+        <v>765</v>
       </c>
       <c r="C257" t="s">
-        <v>740</v>
+        <v>766</v>
       </c>
       <c r="D257" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F257" t="s">
         <v>10</v>
@@ -7242,16 +7413,16 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" t="s">
-        <v>741</v>
+        <v>767</v>
       </c>
       <c r="B258" t="s">
-        <v>742</v>
+        <v>768</v>
       </c>
       <c r="C258" t="s">
-        <v>743</v>
+        <v>769</v>
       </c>
       <c r="D258" t="s">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="F258" t="s">
         <v>10</v>
@@ -7259,13 +7430,13 @@
     </row>
     <row r="259" spans="1:6">
       <c r="A259" t="s">
-        <v>744</v>
+        <v>770</v>
       </c>
       <c r="B259" t="s">
-        <v>745</v>
+        <v>771</v>
       </c>
       <c r="D259" t="s">
-        <v>746</v>
+        <v>772</v>
       </c>
       <c r="F259" t="s">
         <v>10</v>
@@ -7273,16 +7444,16 @@
     </row>
     <row r="260" spans="1:6">
       <c r="A260" t="s">
-        <v>747</v>
+        <v>773</v>
       </c>
       <c r="B260" t="s">
-        <v>748</v>
+        <v>774</v>
       </c>
       <c r="C260" t="s">
-        <v>749</v>
+        <v>775</v>
       </c>
       <c r="D260" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F260" t="s">
         <v>10</v>
@@ -7290,16 +7461,16 @@
     </row>
     <row r="261" spans="1:6">
       <c r="A261" t="s">
-        <v>751</v>
+        <v>777</v>
       </c>
       <c r="B261" t="s">
-        <v>752</v>
+        <v>778</v>
       </c>
       <c r="C261" t="s">
-        <v>753</v>
+        <v>779</v>
       </c>
       <c r="D261" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F261" t="s">
         <v>10</v>
@@ -7307,16 +7478,16 @@
     </row>
     <row r="262" spans="1:6">
       <c r="A262" t="s">
-        <v>754</v>
+        <v>780</v>
       </c>
       <c r="B262" t="s">
-        <v>755</v>
+        <v>781</v>
       </c>
       <c r="C262" t="s">
-        <v>756</v>
+        <v>782</v>
       </c>
       <c r="D262" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F262" t="s">
         <v>10</v>
@@ -7324,16 +7495,16 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" t="s">
-        <v>757</v>
+        <v>783</v>
       </c>
       <c r="B263" t="s">
-        <v>758</v>
+        <v>784</v>
       </c>
       <c r="C263" t="s">
-        <v>759</v>
+        <v>785</v>
       </c>
       <c r="D263" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F263" t="s">
         <v>10</v>
@@ -7341,16 +7512,16 @@
     </row>
     <row r="264" spans="1:6">
       <c r="A264" t="s">
-        <v>760</v>
+        <v>786</v>
       </c>
       <c r="B264" t="s">
-        <v>761</v>
+        <v>787</v>
       </c>
       <c r="C264" t="s">
-        <v>762</v>
+        <v>788</v>
       </c>
       <c r="D264" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F264" t="s">
         <v>195</v>
@@ -7358,13 +7529,13 @@
     </row>
     <row r="265" spans="1:6">
       <c r="A265" t="s">
-        <v>763</v>
+        <v>789</v>
       </c>
       <c r="B265" t="s">
-        <v>764</v>
+        <v>790</v>
       </c>
       <c r="D265" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F265" t="s">
         <v>10</v>
@@ -7372,16 +7543,16 @@
     </row>
     <row r="266" spans="1:6">
       <c r="A266" t="s">
-        <v>765</v>
+        <v>791</v>
       </c>
       <c r="B266" t="s">
-        <v>766</v>
+        <v>792</v>
       </c>
       <c r="C266" t="s">
-        <v>767</v>
+        <v>793</v>
       </c>
       <c r="D266" t="s">
-        <v>750</v>
+        <v>776</v>
       </c>
       <c r="F266" t="s">
         <v>10</v>
@@ -7389,13 +7560,13 @@
     </row>
     <row r="267" spans="1:6">
       <c r="A267" t="s">
-        <v>768</v>
+        <v>794</v>
       </c>
       <c r="B267" t="s">
-        <v>769</v>
+        <v>795</v>
       </c>
       <c r="D267" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F267" t="s">
         <v>10</v>
@@ -7403,16 +7574,16 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" t="s">
-        <v>771</v>
+        <v>797</v>
       </c>
       <c r="B268" t="s">
-        <v>772</v>
+        <v>798</v>
       </c>
       <c r="C268" t="s">
-        <v>773</v>
+        <v>799</v>
       </c>
       <c r="D268" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F268" t="s">
         <v>10</v>
@@ -7420,16 +7591,16 @@
     </row>
     <row r="269" spans="1:6">
       <c r="A269" t="s">
-        <v>774</v>
+        <v>800</v>
       </c>
       <c r="B269" t="s">
-        <v>775</v>
+        <v>801</v>
       </c>
       <c r="C269" t="s">
-        <v>776</v>
+        <v>802</v>
       </c>
       <c r="D269" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F269" t="s">
         <v>10</v>
@@ -7437,16 +7608,16 @@
     </row>
     <row r="270" spans="1:6">
       <c r="A270" t="s">
-        <v>777</v>
+        <v>803</v>
       </c>
       <c r="B270" t="s">
-        <v>778</v>
+        <v>804</v>
       </c>
       <c r="C270" t="s">
-        <v>779</v>
+        <v>805</v>
       </c>
       <c r="D270" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F270" t="s">
         <v>10</v>
@@ -7454,16 +7625,16 @@
     </row>
     <row r="271" spans="1:6">
       <c r="A271" t="s">
-        <v>780</v>
+        <v>806</v>
       </c>
       <c r="B271" t="s">
-        <v>781</v>
+        <v>807</v>
       </c>
       <c r="C271" t="s">
-        <v>782</v>
+        <v>808</v>
       </c>
       <c r="D271" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F271" t="s">
         <v>10</v>
@@ -7471,16 +7642,16 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" t="s">
-        <v>783</v>
+        <v>809</v>
       </c>
       <c r="B272" t="s">
-        <v>784</v>
+        <v>810</v>
       </c>
       <c r="C272" t="s">
-        <v>785</v>
+        <v>811</v>
       </c>
       <c r="D272" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F272" t="s">
         <v>10</v>
@@ -7488,16 +7659,16 @@
     </row>
     <row r="273" spans="1:6">
       <c r="A273" t="s">
-        <v>786</v>
+        <v>812</v>
       </c>
       <c r="B273" t="s">
-        <v>781</v>
+        <v>807</v>
       </c>
       <c r="C273" t="s">
-        <v>787</v>
+        <v>813</v>
       </c>
       <c r="D273" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F273" t="s">
         <v>10</v>
@@ -7505,16 +7676,16 @@
     </row>
     <row r="274" spans="1:6">
       <c r="A274" t="s">
-        <v>788</v>
+        <v>814</v>
       </c>
       <c r="B274" t="s">
-        <v>789</v>
+        <v>815</v>
       </c>
       <c r="C274" t="s">
-        <v>790</v>
+        <v>816</v>
       </c>
       <c r="D274" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F274" t="s">
         <v>10</v>
@@ -7522,16 +7693,16 @@
     </row>
     <row r="275" spans="1:6">
       <c r="A275" t="s">
-        <v>791</v>
+        <v>817</v>
       </c>
       <c r="B275" t="s">
-        <v>792</v>
+        <v>818</v>
       </c>
       <c r="C275" t="s">
-        <v>793</v>
+        <v>819</v>
       </c>
       <c r="D275" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F275" t="s">
         <v>10</v>
@@ -7539,13 +7710,13 @@
     </row>
     <row r="276" spans="1:6">
       <c r="A276" t="s">
-        <v>794</v>
+        <v>820</v>
       </c>
       <c r="B276" t="s">
-        <v>795</v>
+        <v>821</v>
       </c>
       <c r="D276" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F276" t="s">
         <v>10</v>
@@ -7553,13 +7724,13 @@
     </row>
     <row r="277" spans="1:6">
       <c r="A277" t="s">
+        <v>822</v>
+      </c>
+      <c r="B277" t="s">
+        <v>823</v>
+      </c>
+      <c r="D277" t="s">
         <v>796</v>
-      </c>
-      <c r="B277" t="s">
-        <v>797</v>
-      </c>
-      <c r="D277" t="s">
-        <v>770</v>
       </c>
       <c r="F277" t="s">
         <v>10</v>
@@ -7567,13 +7738,13 @@
     </row>
     <row r="278" spans="1:6">
       <c r="A278" t="s">
-        <v>798</v>
+        <v>824</v>
       </c>
       <c r="B278" t="s">
-        <v>799</v>
+        <v>825</v>
       </c>
       <c r="D278" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F278" t="s">
         <v>10</v>
@@ -7581,16 +7752,16 @@
     </row>
     <row r="279" spans="1:6">
       <c r="A279" t="s">
-        <v>800</v>
+        <v>826</v>
       </c>
       <c r="B279" t="s">
-        <v>801</v>
+        <v>827</v>
       </c>
       <c r="C279" t="s">
-        <v>802</v>
+        <v>828</v>
       </c>
       <c r="D279" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F279" t="s">
         <v>10</v>
@@ -7598,16 +7769,16 @@
     </row>
     <row r="280" spans="1:6">
       <c r="A280" t="s">
-        <v>803</v>
+        <v>829</v>
       </c>
       <c r="B280" t="s">
-        <v>804</v>
+        <v>830</v>
       </c>
       <c r="C280" t="s">
-        <v>805</v>
+        <v>831</v>
       </c>
       <c r="D280" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
       <c r="F280" t="s">
         <v>10</v>
@@ -7615,16 +7786,16 @@
     </row>
     <row r="281" spans="1:6">
       <c r="A281" t="s">
-        <v>806</v>
+        <v>832</v>
       </c>
       <c r="B281" t="s">
-        <v>807</v>
+        <v>833</v>
       </c>
       <c r="C281" t="s">
-        <v>808</v>
+        <v>834</v>
       </c>
       <c r="D281" t="s">
-        <v>809</v>
+        <v>835</v>
       </c>
       <c r="F281" t="s">
         <v>10</v>
@@ -7632,16 +7803,16 @@
     </row>
     <row r="282" spans="1:6">
       <c r="A282" t="s">
-        <v>810</v>
+        <v>836</v>
       </c>
       <c r="B282" t="s">
-        <v>811</v>
+        <v>837</v>
       </c>
       <c r="C282" t="s">
-        <v>812</v>
+        <v>838</v>
       </c>
       <c r="D282" t="s">
-        <v>813</v>
+        <v>839</v>
       </c>
       <c r="F282" t="s">
         <v>10</v>
@@ -7649,16 +7820,16 @@
     </row>
     <row r="283" spans="1:6">
       <c r="A283" t="s">
-        <v>814</v>
+        <v>840</v>
       </c>
       <c r="B283" t="s">
-        <v>815</v>
+        <v>841</v>
       </c>
       <c r="C283" t="s">
-        <v>816</v>
+        <v>842</v>
       </c>
       <c r="D283" t="s">
-        <v>817</v>
+        <v>843</v>
       </c>
       <c r="F283" t="s">
         <v>10</v>
@@ -7666,16 +7837,16 @@
     </row>
     <row r="284" spans="1:6">
       <c r="A284" t="s">
-        <v>818</v>
+        <v>844</v>
       </c>
       <c r="B284" t="s">
-        <v>819</v>
+        <v>845</v>
       </c>
       <c r="C284" t="s">
-        <v>820</v>
+        <v>846</v>
       </c>
       <c r="D284" t="s">
-        <v>817</v>
+        <v>843</v>
       </c>
       <c r="F284" t="s">
         <v>10</v>
@@ -7683,16 +7854,16 @@
     </row>
     <row r="285" spans="1:6">
       <c r="A285" t="s">
-        <v>821</v>
+        <v>847</v>
       </c>
       <c r="B285" t="s">
-        <v>822</v>
+        <v>848</v>
       </c>
       <c r="C285" t="s">
-        <v>823</v>
+        <v>849</v>
       </c>
       <c r="D285" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F285" t="s">
         <v>10</v>
@@ -7700,13 +7871,13 @@
     </row>
     <row r="286" spans="1:6">
       <c r="A286" t="s">
-        <v>825</v>
+        <v>851</v>
       </c>
       <c r="B286" t="s">
-        <v>826</v>
+        <v>852</v>
       </c>
       <c r="D286" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F286" t="s">
         <v>10</v>
@@ -7714,16 +7885,16 @@
     </row>
     <row r="287" spans="1:6">
       <c r="A287" t="s">
-        <v>827</v>
+        <v>853</v>
       </c>
       <c r="B287" t="s">
-        <v>828</v>
+        <v>854</v>
       </c>
       <c r="C287" t="s">
-        <v>829</v>
+        <v>855</v>
       </c>
       <c r="D287" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F287" t="s">
         <v>10</v>
@@ -7731,13 +7902,13 @@
     </row>
     <row r="288" spans="1:6">
       <c r="A288" t="s">
-        <v>830</v>
+        <v>856</v>
       </c>
       <c r="B288" t="s">
-        <v>831</v>
+        <v>857</v>
       </c>
       <c r="D288" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F288" t="s">
         <v>10</v>
@@ -7745,16 +7916,16 @@
     </row>
     <row r="289" spans="1:6">
       <c r="A289" t="s">
-        <v>832</v>
+        <v>858</v>
       </c>
       <c r="B289" t="s">
-        <v>833</v>
+        <v>859</v>
       </c>
       <c r="C289" t="s">
-        <v>834</v>
+        <v>860</v>
       </c>
       <c r="D289" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F289" t="s">
         <v>10</v>
@@ -7762,16 +7933,16 @@
     </row>
     <row r="290" spans="1:6">
       <c r="A290" t="s">
-        <v>835</v>
+        <v>861</v>
       </c>
       <c r="B290" t="s">
-        <v>836</v>
+        <v>862</v>
       </c>
       <c r="C290" t="s">
-        <v>837</v>
+        <v>863</v>
       </c>
       <c r="D290" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F290" t="s">
         <v>10</v>
@@ -7779,16 +7950,16 @@
     </row>
     <row r="291" spans="1:6">
       <c r="A291" t="s">
-        <v>838</v>
+        <v>864</v>
       </c>
       <c r="B291" t="s">
-        <v>839</v>
+        <v>865</v>
       </c>
       <c r="C291" t="s">
-        <v>840</v>
+        <v>866</v>
       </c>
       <c r="D291" t="s">
-        <v>824</v>
+        <v>850</v>
       </c>
       <c r="F291" t="s">
         <v>10</v>
@@ -7796,16 +7967,16 @@
     </row>
     <row r="292" spans="1:6">
       <c r="A292" t="s">
-        <v>841</v>
+        <v>867</v>
       </c>
       <c r="B292" t="s">
-        <v>842</v>
+        <v>868</v>
       </c>
       <c r="C292" t="s">
-        <v>843</v>
+        <v>869</v>
       </c>
       <c r="D292" t="s">
-        <v>844</v>
+        <v>870</v>
       </c>
       <c r="F292" t="s">
         <v>10</v>
@@ -7813,16 +7984,16 @@
     </row>
     <row r="293" spans="1:6">
       <c r="A293" t="s">
-        <v>845</v>
+        <v>871</v>
       </c>
       <c r="B293" t="s">
-        <v>846</v>
+        <v>872</v>
       </c>
       <c r="C293" t="s">
-        <v>847</v>
+        <v>873</v>
       </c>
       <c r="D293" t="s">
-        <v>844</v>
+        <v>870</v>
       </c>
       <c r="F293" t="s">
         <v>10</v>
@@ -7830,16 +8001,16 @@
     </row>
     <row r="294" spans="1:6">
       <c r="A294" t="s">
-        <v>848</v>
+        <v>874</v>
       </c>
       <c r="B294" t="s">
-        <v>849</v>
+        <v>875</v>
       </c>
       <c r="C294" t="s">
-        <v>850</v>
+        <v>876</v>
       </c>
       <c r="D294" t="s">
-        <v>844</v>
+        <v>870</v>
       </c>
       <c r="F294" t="s">
         <v>10</v>
@@ -7847,16 +8018,16 @@
     </row>
     <row r="295" spans="1:6">
       <c r="A295" t="s">
-        <v>851</v>
+        <v>877</v>
       </c>
       <c r="B295" t="s">
-        <v>852</v>
+        <v>878</v>
       </c>
       <c r="C295" t="s">
-        <v>853</v>
+        <v>879</v>
       </c>
       <c r="D295" t="s">
-        <v>854</v>
+        <v>880</v>
       </c>
       <c r="F295" t="s">
         <v>10</v>
@@ -7864,16 +8035,16 @@
     </row>
     <row r="296" spans="1:6">
       <c r="A296" t="s">
-        <v>855</v>
+        <v>881</v>
       </c>
       <c r="B296" t="s">
-        <v>856</v>
+        <v>882</v>
       </c>
       <c r="C296" t="s">
-        <v>857</v>
+        <v>883</v>
       </c>
       <c r="D296" t="s">
-        <v>858</v>
+        <v>884</v>
       </c>
       <c r="F296" t="s">
         <v>195</v>
@@ -7881,16 +8052,16 @@
     </row>
     <row r="297" spans="1:6">
       <c r="A297" t="s">
-        <v>859</v>
+        <v>885</v>
       </c>
       <c r="B297" t="s">
-        <v>860</v>
+        <v>886</v>
       </c>
       <c r="C297" t="s">
-        <v>861</v>
+        <v>887</v>
       </c>
       <c r="D297" t="s">
-        <v>858</v>
+        <v>884</v>
       </c>
       <c r="F297" t="s">
         <v>10</v>
@@ -7898,13 +8069,13 @@
     </row>
     <row r="298" spans="1:6">
       <c r="A298" t="s">
-        <v>862</v>
+        <v>888</v>
       </c>
       <c r="B298" t="s">
-        <v>863</v>
+        <v>889</v>
       </c>
       <c r="D298" t="s">
-        <v>864</v>
+        <v>890</v>
       </c>
       <c r="F298" t="s">
         <v>10</v>
@@ -7912,10 +8083,10 @@
     </row>
     <row r="299" spans="1:6">
       <c r="A299" t="s">
-        <v>865</v>
+        <v>891</v>
       </c>
       <c r="D299" t="s">
-        <v>866</v>
+        <v>892</v>
       </c>
       <c r="F299" t="s">
         <v>195</v>
@@ -7923,10 +8094,10 @@
     </row>
     <row r="300" spans="1:6">
       <c r="A300" t="s">
-        <v>867</v>
+        <v>893</v>
       </c>
       <c r="D300" t="s">
-        <v>866</v>
+        <v>892</v>
       </c>
       <c r="F300" t="s">
         <v>195</v>
@@ -7934,10 +8105,10 @@
     </row>
     <row r="301" spans="1:6">
       <c r="A301" t="s">
-        <v>868</v>
+        <v>894</v>
       </c>
       <c r="D301" t="s">
-        <v>866</v>
+        <v>892</v>
       </c>
       <c r="F301" t="s">
         <v>195</v>
@@ -7945,16 +8116,16 @@
     </row>
     <row r="302" spans="1:6">
       <c r="A302" t="s">
-        <v>869</v>
+        <v>895</v>
       </c>
       <c r="B302" t="s">
-        <v>870</v>
+        <v>896</v>
       </c>
       <c r="C302" t="s">
-        <v>871</v>
+        <v>897</v>
       </c>
       <c r="D302" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F302" t="s">
         <v>10</v>
@@ -7962,16 +8133,16 @@
     </row>
     <row r="303" spans="1:6">
       <c r="A303" t="s">
-        <v>873</v>
+        <v>899</v>
       </c>
       <c r="B303" t="s">
-        <v>874</v>
+        <v>900</v>
       </c>
       <c r="C303" t="s">
-        <v>875</v>
+        <v>901</v>
       </c>
       <c r="D303" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F303" t="s">
         <v>10</v>
@@ -7979,16 +8150,16 @@
     </row>
     <row r="304" spans="1:6">
       <c r="A304" t="s">
-        <v>876</v>
+        <v>902</v>
       </c>
       <c r="B304" t="s">
-        <v>877</v>
+        <v>903</v>
       </c>
       <c r="C304" t="s">
-        <v>878</v>
+        <v>904</v>
       </c>
       <c r="D304" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F304" t="s">
         <v>10</v>
@@ -7996,16 +8167,16 @@
     </row>
     <row r="305" spans="1:6">
       <c r="A305" t="s">
-        <v>879</v>
+        <v>905</v>
       </c>
       <c r="B305" t="s">
-        <v>880</v>
+        <v>906</v>
       </c>
       <c r="C305" t="s">
-        <v>881</v>
+        <v>907</v>
       </c>
       <c r="D305" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F305" t="s">
         <v>10</v>
@@ -8013,16 +8184,16 @@
     </row>
     <row r="306" spans="1:6">
       <c r="A306" t="s">
-        <v>882</v>
+        <v>908</v>
       </c>
       <c r="B306" t="s">
-        <v>883</v>
+        <v>909</v>
       </c>
       <c r="C306" t="s">
-        <v>884</v>
+        <v>910</v>
       </c>
       <c r="D306" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F306" t="s">
         <v>10</v>
@@ -8030,16 +8201,16 @@
     </row>
     <row r="307" spans="1:6">
       <c r="A307" t="s">
-        <v>885</v>
+        <v>911</v>
       </c>
       <c r="B307" t="s">
-        <v>886</v>
+        <v>912</v>
       </c>
       <c r="C307" t="s">
-        <v>887</v>
+        <v>913</v>
       </c>
       <c r="D307" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F307" t="s">
         <v>10</v>
@@ -8047,16 +8218,16 @@
     </row>
     <row r="308" spans="1:6">
       <c r="A308" t="s">
-        <v>888</v>
+        <v>914</v>
       </c>
       <c r="B308" t="s">
-        <v>889</v>
+        <v>915</v>
       </c>
       <c r="C308" t="s">
-        <v>890</v>
+        <v>916</v>
       </c>
       <c r="D308" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F308" t="s">
         <v>10</v>
@@ -8064,16 +8235,16 @@
     </row>
     <row r="309" spans="1:6">
       <c r="A309" t="s">
-        <v>891</v>
+        <v>917</v>
       </c>
       <c r="B309" t="s">
-        <v>892</v>
+        <v>918</v>
       </c>
       <c r="C309" t="s">
-        <v>893</v>
+        <v>919</v>
       </c>
       <c r="D309" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F309" t="s">
         <v>10</v>
@@ -8081,16 +8252,16 @@
     </row>
     <row r="310" spans="1:6">
       <c r="A310" t="s">
-        <v>894</v>
+        <v>920</v>
       </c>
       <c r="B310" t="s">
-        <v>895</v>
+        <v>921</v>
       </c>
       <c r="C310" t="s">
-        <v>896</v>
+        <v>922</v>
       </c>
       <c r="D310" t="s">
-        <v>872</v>
+        <v>898</v>
       </c>
       <c r="F310" t="s">
         <v>10</v>
@@ -8098,16 +8269,16 @@
     </row>
     <row r="311" spans="1:6">
       <c r="A311" t="s">
-        <v>897</v>
+        <v>923</v>
       </c>
       <c r="B311" t="s">
-        <v>898</v>
+        <v>924</v>
       </c>
       <c r="C311" t="s">
-        <v>899</v>
+        <v>925</v>
       </c>
       <c r="D311" t="s">
-        <v>900</v>
+        <v>926</v>
       </c>
       <c r="F311" t="s">
         <v>10</v>
@@ -8115,16 +8286,16 @@
     </row>
     <row r="312" spans="1:6">
       <c r="A312" t="s">
-        <v>901</v>
+        <v>927</v>
       </c>
       <c r="B312" t="s">
-        <v>902</v>
+        <v>928</v>
       </c>
       <c r="C312" t="s">
-        <v>903</v>
+        <v>929</v>
       </c>
       <c r="D312" t="s">
-        <v>900</v>
+        <v>926</v>
       </c>
       <c r="F312" t="s">
         <v>10</v>

</xml_diff>